<commit_message>
updates the regex to only get the text between the <>
</commit_message>
<xml_diff>
--- a/Locked Excel Workbook.xlsx
+++ b/Locked Excel Workbook.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bowdenb\PycharmProjects\UnprotectExcelWorksheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Blake\PycharmProjects\UnprotectExcelWorksheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8614EC-3B24-4069-BA80-5476324C057F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66FF9638-5A70-4AD5-9CFA-553F305B2635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -355,7 +355,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -377,7 +377,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -396,7 +396,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A8ACDB0-A970-44E9-916C-78994829B471}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>